<commit_message>
add single buffers to signal output, update layout
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pengyuan\Desktop\FYP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88740BE-3860-431A-A5DC-B22F63E732DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079898B0-5A66-4AC4-B6EF-D8C91F0A19E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="73">
   <si>
     <t>Models</t>
   </si>
@@ -309,6 +309,14 @@
   </si>
   <si>
     <t>LAUNCHXL-F28379D</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Single buffer (non-inverting)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SN74LV1T34DBVRG4</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -791,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1108,7 +1116,7 @@
         <v>2.66</v>
       </c>
       <c r="H14" s="3">
-        <f t="shared" ref="H14:H30" si="1">G14*F14</f>
+        <f t="shared" ref="H14:H31" si="1">G14*F14</f>
         <v>31.92</v>
       </c>
     </row>
@@ -1138,130 +1146,130 @@
     </row>
     <row r="16" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="8">
+        <v>3</v>
+      </c>
+      <c r="G16" s="8">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="H16" s="3">
+        <f t="shared" si="1"/>
+        <v>0.873</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C17" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D17" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E17" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F17" s="8">
         <v>12</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G17" s="13">
         <v>9.1199999999999992</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H17" s="13">
         <f t="shared" si="1"/>
         <v>109.44</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="7" t="s">
+    <row r="18" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C18" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D18" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E18" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F18" s="8">
         <v>12</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G18" s="8">
         <v>0.1</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H18" s="3">
         <f t="shared" si="1"/>
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="2" t="s">
+    <row r="19" spans="2:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D19" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F19" s="3">
         <v>2</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G19" s="3">
         <v>3.06</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H19" s="3">
         <f t="shared" si="1"/>
         <v>6.12</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="7" t="s">
+    <row r="20" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C20" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D20" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E20" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F20" s="8">
         <v>3</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G20" s="8">
         <v>0.22</v>
-      </c>
-      <c r="H19" s="13">
-        <f>G19*F19</f>
-        <v>0.66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F20" s="8">
-        <v>5</v>
-      </c>
-      <c r="G20" s="8">
-        <v>0.11</v>
       </c>
       <c r="H20" s="13">
         <f>G20*F20</f>
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>48</v>
@@ -1270,286 +1278,294 @@
         <v>49</v>
       </c>
       <c r="F21" s="8">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="G21" s="8">
-        <v>0.08</v>
+        <v>0.11</v>
       </c>
       <c r="H21" s="13">
         <f>G21*F21</f>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="8">
+        <v>80</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0.08</v>
+      </c>
+      <c r="H22" s="13">
+        <f>G22*F22</f>
         <v>6.4</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="7" t="s">
+    <row r="23" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C23" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D23" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E23" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F23" s="8">
         <v>2</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G23" s="13">
         <v>5.3</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H23" s="13">
         <f t="shared" si="1"/>
         <v>10.6</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="7" t="s">
+    <row r="24" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C24" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D24" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E24" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F24" s="8">
         <v>36</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G24" s="8">
         <v>0.08</v>
       </c>
-      <c r="H23" s="13">
+      <c r="H24" s="13">
         <f t="shared" si="1"/>
         <v>2.88</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="7" t="s">
+    <row r="25" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C25" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D25" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E25" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F25" s="8">
         <v>24</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G25" s="8">
         <v>0.08</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H25" s="13">
         <f t="shared" si="1"/>
         <v>1.92</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="7" t="s">
+    <row r="26" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C26" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F25" s="8">
-        <v>3</v>
-      </c>
-      <c r="G25" s="8">
-        <v>0.08</v>
-      </c>
-      <c r="H25" s="13">
-        <f>G25*F25</f>
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="8">
-        <v>1714971</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>48</v>
       </c>
       <c r="E26" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="8">
+        <v>3</v>
+      </c>
+      <c r="G26" s="8">
+        <v>0.08</v>
+      </c>
+      <c r="H26" s="13">
+        <f>G26*F26</f>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="8">
+        <v>1714971</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F27" s="8">
         <v>2</v>
       </c>
-      <c r="G26" s="8">
+      <c r="G27" s="8">
         <v>1.39</v>
       </c>
-      <c r="H26" s="13">
+      <c r="H27" s="13">
         <f t="shared" si="1"/>
         <v>2.78</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="7" t="s">
+    <row r="28" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C28" s="8">
         <v>1714984</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D28" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E28" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F28" s="8">
         <v>1</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G28" s="8">
         <v>2.04</v>
       </c>
-      <c r="H27" s="13">
+      <c r="H28" s="13">
         <f t="shared" si="1"/>
         <v>2.04</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="2" t="s">
+    <row r="29" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C29" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D29" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E29" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F29" s="8">
         <v>3</v>
       </c>
-      <c r="G28" s="8">
+      <c r="G29" s="8">
         <v>17.29</v>
       </c>
-      <c r="H28" s="13">
+      <c r="H29" s="13">
         <f t="shared" si="1"/>
         <v>51.87</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="7" t="s">
+    <row r="30" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C30" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D30" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E30" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F30" s="8">
         <v>12</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G30" s="8">
         <v>17.059999999999999</v>
       </c>
-      <c r="H29" s="13">
+      <c r="H30" s="13">
         <f t="shared" si="1"/>
         <v>204.71999999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="2" t="s">
+    <row r="31" spans="2:8" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F31" s="3">
         <v>3</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G31" s="3">
         <v>4.8</v>
       </c>
-      <c r="H30" s="13">
+      <c r="H31" s="13">
         <f t="shared" si="1"/>
         <v>14.399999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-    </row>
-    <row r="32" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="11" t="s">
+    <row r="32" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+    </row>
+    <row r="33" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B33" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C33" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D33" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E33" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F33" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="G33" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="H33" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="7" t="s">
+    <row r="34" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8">
-        <v>3</v>
-      </c>
-      <c r="G33" s="8"/>
-      <c r="H33" s="13">
-        <f t="shared" ref="H33:H35" si="2">G33*F33</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
@@ -1559,43 +1575,59 @@
       </c>
       <c r="G34" s="8"/>
       <c r="H34" s="13">
+        <f t="shared" ref="H34:H36" si="2">G34*F34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8">
+        <v>3</v>
+      </c>
+      <c r="G35" s="8"/>
+      <c r="H35" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="7" t="s">
+    <row r="36" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C36" s="8">
         <v>1714984</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D36" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E36" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="8">
+      <c r="F36" s="8">
         <v>1</v>
       </c>
-      <c r="G35" s="8">
+      <c r="G36" s="8">
         <v>2.04</v>
       </c>
-      <c r="H35" s="13">
+      <c r="H36" s="13">
         <f t="shared" si="2"/>
         <v>2.04</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="12" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="11">
-        <f>SUM(H4:H9)+SUM(H12:H30)+SUM(H33:H35)</f>
-        <v>808.39999999999986</v>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="11">
+        <f>SUM(H4:H9)+SUM(H12:H31)+SUM(H34:H36)</f>
+        <v>809.27299999999991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified single buffer to voltage follower, modification on gate drive protection circuit is needed
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pengyuan\Desktop\FYP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079898B0-5A66-4AC4-B6EF-D8C91F0A19E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6827ABAC-92E5-4DFD-A7D5-0E3CCA48F57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="73">
   <si>
     <t>Models</t>
   </si>
@@ -60,10 +60,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>HVCB0603FDC100M</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Mouser</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -281,10 +277,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>100M resistor</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>10 ohm resistor</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -316,7 +308,15 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>SN74LV1T34DBVRG4</t>
+    <t>20k resistor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>6 pin terminal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>6 pin screw plug</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -799,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -822,10 +822,10 @@
     </row>
     <row r="2" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>0</v>
@@ -834,53 +834,53 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C4" s="8">
         <v>1714971</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" s="8">
         <v>2</v>
@@ -889,537 +889,490 @@
         <v>1.39</v>
       </c>
       <c r="H4" s="13">
-        <f t="shared" ref="H4:H6" si="0">G4*F4</f>
+        <f t="shared" ref="H4:H7" si="0">G4*F4</f>
         <v>2.78</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="3">
+      <c r="B5" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="13"/>
+    </row>
+    <row r="6" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="13"/>
+    </row>
+    <row r="7" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="3">
         <v>12</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G7" s="8">
         <v>17.29</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H7" s="13">
         <f t="shared" si="0"/>
         <v>207.48</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="3">
-        <v>3</v>
-      </c>
-      <c r="G6" s="8">
-        <v>17.059999999999999</v>
-      </c>
-      <c r="H6" s="13">
-        <f t="shared" si="0"/>
-        <v>51.179999999999993</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="8">
-        <v>12</v>
-      </c>
-      <c r="G7" s="8">
-        <v>0.08</v>
-      </c>
-      <c r="H7" s="13">
-        <f>G7*F7</f>
-        <v>0.96</v>
-      </c>
-    </row>
     <row r="8" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="C8" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="E8" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="F8" s="8">
         <v>12</v>
       </c>
       <c r="G8" s="8">
-        <v>0.11</v>
+        <v>0.08</v>
       </c>
       <c r="H8" s="13">
         <f>G8*F8</f>
-        <v>1.32</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D9" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>49</v>
-      </c>
       <c r="F9" s="8">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G9" s="8">
-        <v>0.08</v>
+        <v>0.11</v>
       </c>
       <c r="H9" s="13">
         <f>G9*F9</f>
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="8">
+        <v>5</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0.08</v>
+      </c>
+      <c r="H10" s="13">
+        <f>G10*F10</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-    </row>
-    <row r="11" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="6" t="s">
+    <row r="11" spans="1:8" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+    </row>
+    <row r="12" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="6" t="s">
+      <c r="E12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
+      <c r="E13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="3">
         <v>12</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="3">
-        <v>12</v>
-      </c>
-      <c r="G12" s="9">
+      <c r="G13" s="9">
         <v>3.75</v>
-      </c>
-      <c r="H12" s="3">
-        <f>G12*F12</f>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="8">
-        <v>18</v>
-      </c>
-      <c r="G13" s="8">
-        <v>1.75</v>
       </c>
       <c r="H13" s="3">
         <f>G13*F13</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="8">
+        <v>18</v>
+      </c>
+      <c r="G14" s="8">
+        <v>1.75</v>
+      </c>
+      <c r="H14" s="3">
+        <f>G14*F14</f>
         <v>31.5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="2" t="s">
+    <row r="15" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="C15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="3">
+      <c r="E15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="3">
         <v>12</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G15" s="3">
         <v>2.66</v>
       </c>
-      <c r="H14" s="3">
-        <f t="shared" ref="H14:H31" si="1">G14*F14</f>
+      <c r="H15" s="3">
+        <f t="shared" ref="H15:H32" si="1">G15*F15</f>
         <v>31.92</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="8" t="s">
+    <row r="16" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="C16" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="8">
+      <c r="F16" s="8">
         <v>12</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G16" s="8">
         <v>1.5</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H16" s="3">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="8">
-        <v>3</v>
-      </c>
-      <c r="G16" s="8">
-        <v>0.29099999999999998</v>
-      </c>
-      <c r="H16" s="3">
-        <f t="shared" si="1"/>
-        <v>0.873</v>
-      </c>
-    </row>
     <row r="17" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8">
+        <v>3</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="8">
+      <c r="E18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="8">
         <v>12</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G18" s="13">
         <v>9.1199999999999992</v>
       </c>
-      <c r="H17" s="13">
+      <c r="H18" s="13">
         <f t="shared" si="1"/>
         <v>109.44</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="8" t="s">
+    <row r="19" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" s="8">
+      <c r="F19" s="8">
         <v>12</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G19" s="8">
         <v>0.1</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H19" s="3">
         <f t="shared" si="1"/>
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="3">
+    <row r="20" spans="2:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="3">
         <v>2</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G20" s="3">
         <v>3.06</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H20" s="3">
         <f t="shared" si="1"/>
         <v>6.12</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F20" s="8">
-        <v>3</v>
-      </c>
-      <c r="G20" s="8">
-        <v>0.22</v>
-      </c>
-      <c r="H20" s="13">
-        <f>G20*F20</f>
-        <v>0.66</v>
-      </c>
-    </row>
     <row r="21" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>49</v>
       </c>
       <c r="F21" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G21" s="8">
-        <v>0.11</v>
+        <v>0.22</v>
       </c>
       <c r="H21" s="13">
         <f>G21*F21</f>
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D22" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>49</v>
-      </c>
       <c r="F22" s="8">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="G22" s="8">
-        <v>0.08</v>
+        <v>0.11</v>
       </c>
       <c r="H22" s="13">
         <f>G22*F22</f>
-        <v>6.4</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="7" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F23" s="8">
-        <v>2</v>
-      </c>
-      <c r="G23" s="13">
-        <v>5.3</v>
+        <v>80</v>
+      </c>
+      <c r="G23" s="8">
+        <v>0.08</v>
       </c>
       <c r="H23" s="13">
-        <f t="shared" si="1"/>
-        <v>10.6</v>
+        <f>G23*F23</f>
+        <v>6.4</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F24" s="8">
+        <v>70</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+    </row>
+    <row r="25" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" s="8">
         <v>36</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G25" s="8">
         <v>0.08</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H25" s="13">
         <f t="shared" si="1"/>
         <v>2.88</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F25" s="8">
+    <row r="26" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="8">
         <v>24</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G26" s="8">
         <v>0.08</v>
       </c>
-      <c r="H25" s="13">
+      <c r="H26" s="13">
         <f t="shared" si="1"/>
         <v>1.92</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F26" s="8">
-        <v>3</v>
-      </c>
-      <c r="G26" s="8">
-        <v>0.08</v>
-      </c>
-      <c r="H26" s="13">
-        <f>G26*F26</f>
-        <v>0.24</v>
-      </c>
-    </row>
     <row r="27" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C27" s="8">
         <v>1714971</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F27" s="8">
         <v>2</v>
@@ -1434,16 +1387,16 @@
     </row>
     <row r="28" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C28" s="8">
         <v>1714984</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F28" s="8">
         <v>1</v>
@@ -1457,126 +1410,134 @@
       </c>
     </row>
     <row r="29" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>68</v>
+      <c r="B29" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="8">
+        <v>1827907</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F29" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G29" s="8">
-        <v>17.29</v>
+        <v>2.88</v>
       </c>
       <c r="H29" s="13">
         <f t="shared" si="1"/>
-        <v>51.87</v>
+        <v>2.88</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>69</v>
+        <v>72</v>
+      </c>
+      <c r="C30" s="8">
+        <v>1827745</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F30" s="8">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="G30" s="8">
-        <v>17.059999999999999</v>
+        <v>4.91</v>
       </c>
       <c r="H30" s="13">
         <f t="shared" si="1"/>
-        <v>204.71999999999997</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F31" s="3">
-        <v>3</v>
-      </c>
-      <c r="G31" s="3">
-        <v>4.8</v>
+        <v>4.91</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31" s="8">
+        <v>12</v>
+      </c>
+      <c r="G31" s="8">
+        <v>17.059999999999999</v>
       </c>
       <c r="H31" s="13">
         <f t="shared" si="1"/>
+        <v>204.71999999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F32" s="3">
+        <v>3</v>
+      </c>
+      <c r="G32" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="H32" s="13">
+        <f t="shared" si="1"/>
         <v>14.399999999999999</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-    </row>
     <row r="33" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="11" t="s">
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+    </row>
+    <row r="34" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H34" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8">
-        <v>3</v>
-      </c>
-      <c r="G34" s="8"/>
-      <c r="H34" s="13">
-        <f t="shared" ref="H34:H36" si="2">G34*F34</f>
-        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
@@ -1591,43 +1552,59 @@
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="13">
+        <f t="shared" ref="H35:H37" si="2">G35*F35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8">
+        <v>3</v>
+      </c>
+      <c r="G36" s="8"/>
+      <c r="H36" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C36" s="8">
+    <row r="37" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="8">
         <v>1714984</v>
       </c>
-      <c r="D36" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F36" s="8">
+      <c r="D37" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F37" s="8">
         <v>1</v>
       </c>
-      <c r="G36" s="8">
+      <c r="G37" s="8">
         <v>2.04</v>
       </c>
-      <c r="H36" s="13">
+      <c r="H37" s="13">
         <f t="shared" si="2"/>
         <v>2.04</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="11">
-        <f>SUM(H4:H9)+SUM(H12:H31)+SUM(H34:H36)</f>
-        <v>809.27299999999991</v>
+      <c r="B39" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="11">
+        <f>SUM(H4:H10)+SUM(H13:H32)+SUM(H35:H37)</f>
+        <v>702.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TBC: change trace for 10A current to filled zone
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pengyuan\Desktop\FYP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6827ABAC-92E5-4DFD-A7D5-0E3CCA48F57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8846B004-9265-43BA-A6B5-589E6620B95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="83">
   <si>
     <t>Models</t>
   </si>
@@ -180,143 +180,185 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>TI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMD:SOT-23-5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TMH 0515D</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRACO POWER</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BC846</t>
+  </si>
+  <si>
+    <t>Nexperia</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMD:CP_Elec_16x17.5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CGA2B3X7R1V104K050BB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DigiKey</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMD:0402</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMD:0603</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>THT:TO-3P-3_Vertical</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMD:DIP-8_W8.89mm_LongPads</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C0402C105K9PAC7867</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RMCF0603FT10R0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RMCF0603FT270R</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>06036A102JAT4A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SN74LVC1G04-EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Single invering buffer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fiber-Optic Transmitter</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fiber-Optic Receiver</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.7k ohm resistor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RMCF0603FT4K70</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>10 ohm resistor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>270 ohm resistor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>400V capacitor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>600V 2 pin screw</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AFBR-1624Z</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AFBR-2624Z</t>
+  </si>
+  <si>
+    <t>LAUNCHXL-F28379D</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>20k resistor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>6 pin terminal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>6 pin screw plug</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Operational Amplifier</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zener Diode</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>50 ohm resistor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>100 ohm resistor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>600V 1 pin terminal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2606-1101</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>594-MCT06030E2002BP5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>603-RT0603BRE0750RL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>652-CRT0603BY1000ELF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LMV641MF/NOPB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>78-BZX384C18-G3-18</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>SMD:TO-263-2</t>
-  </si>
-  <si>
-    <t>TI</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SMD:SOT-23-5</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TMH 0515D</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TRACO POWER</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BC846</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>SMD:SOT-23</t>
-  </si>
-  <si>
-    <t>Nexperia</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SMD:CP_Elec_16x17.5</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CGA2B3X7R1V104K050BB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DigiKey</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SMD:0402</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SMD:0603</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>THT:TO-3P-3_Vertical</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SMD:DIP-8_W8.89mm_LongPads</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>C0402C105K9PAC7867</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>RMCF0603FT10R0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>RMCF0603FT270R</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>06036A102JAT4A</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SN74LVC1G04-EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Single invering buffer</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fiber-Optic Transmitter</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fiber-Optic Receiver</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.7k ohm resistor</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>RMCF0603FT4K70</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>10 ohm resistor</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>270 ohm resistor</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>400V capacitor</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>600V 2 pin screw</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>AFBR-1624Z</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>AFBR-2624Z</t>
-  </si>
-  <si>
-    <t>LAUNCHXL-F28379D</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Single buffer (non-inverting)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>20k resistor</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>6 pin terminal</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>6 pin screw plug</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -327,7 +369,7 @@
   <numFmts count="1">
     <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,6 +421,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -482,7 +530,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -517,6 +565,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -799,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -851,7 +905,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>2</v>
@@ -871,13 +925,13 @@
     </row>
     <row r="4" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C4" s="8">
         <v>1714971</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>27</v>
@@ -895,62 +949,88 @@
     </row>
     <row r="5" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="13"/>
+        <v>68</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1827907</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1</v>
+      </c>
+      <c r="G5" s="8">
+        <v>2.88</v>
+      </c>
+      <c r="H5" s="13">
+        <f t="shared" si="0"/>
+        <v>2.88</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="13"/>
+        <v>69</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1827745</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="8">
+        <v>1</v>
+      </c>
+      <c r="G6" s="8">
+        <v>4.91</v>
+      </c>
+      <c r="H6" s="13">
+        <f t="shared" si="0"/>
+        <v>4.91</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="B7" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="15">
         <v>12</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="15">
         <v>17.29</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="15">
         <f t="shared" si="0"/>
         <v>207.48</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F8" s="8">
         <v>12</v>
@@ -968,13 +1048,13 @@
         <v>17</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>48</v>
       </c>
       <c r="F9" s="8">
         <v>12</v>
@@ -992,13 +1072,13 @@
         <v>19</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F10" s="8">
         <v>5</v>
@@ -1057,7 +1137,7 @@
         <v>16</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F13" s="3">
         <v>12</v>
@@ -1081,7 +1161,7 @@
         <v>14</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="F14" s="8">
         <v>18</v>
@@ -1094,237 +1174,258 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="2" t="s">
+    <row r="15" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="8">
+        <v>24</v>
+      </c>
+      <c r="G15" s="8">
+        <v>0.22</v>
+      </c>
+      <c r="H15" s="3">
+        <f>G15*F15</f>
+        <v>5.28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="3">
+      <c r="E16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="3">
         <v>12</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G16" s="3">
         <v>2.66</v>
       </c>
-      <c r="H15" s="3">
-        <f t="shared" ref="H15:H32" si="1">G15*F15</f>
+      <c r="H16" s="3">
+        <f t="shared" ref="H16:H36" si="1">G16*F16</f>
         <v>31.92</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="8" t="s">
+    <row r="17" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="8">
+      <c r="F17" s="8">
         <v>12</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G17" s="8">
         <v>1.5</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H17" s="3">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8">
-        <v>3</v>
-      </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
     <row r="18" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="8">
+        <v>3</v>
+      </c>
+      <c r="G18" s="8">
+        <v>1.96</v>
+      </c>
+      <c r="H18" s="3">
+        <f t="shared" si="1"/>
+        <v>5.88</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C19" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="8" t="s">
+      <c r="E19" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F19" s="15">
         <v>12</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G19" s="15">
         <v>9.1199999999999992</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H19" s="15">
         <f t="shared" si="1"/>
         <v>109.44</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="7" t="s">
+    <row r="20" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C20" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F19" s="8">
+      <c r="E20" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" s="8">
         <v>12</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G20" s="8">
         <v>0.1</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H20" s="3">
         <f t="shared" si="1"/>
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="3" t="s">
+    <row r="21" spans="2:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D21" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" s="3">
+      <c r="E21" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="3">
         <v>2</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G21" s="3">
         <v>3.06</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H21" s="3">
         <f t="shared" si="1"/>
         <v>6.12</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F21" s="8">
-        <v>3</v>
-      </c>
-      <c r="G21" s="8">
-        <v>0.22</v>
-      </c>
-      <c r="H21" s="13">
-        <f>G21*F21</f>
-        <v>0.66</v>
-      </c>
-    </row>
     <row r="22" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="7" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>48</v>
-      </c>
       <c r="F22" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G22" s="8">
-        <v>0.11</v>
+        <v>0.22</v>
       </c>
       <c r="H22" s="13">
         <f>G22*F22</f>
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F23" s="8">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="G23" s="8">
-        <v>0.08</v>
+        <v>0.11</v>
       </c>
       <c r="H23" s="13">
         <f>G23*F23</f>
-        <v>6.4</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
+        <v>19</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="8">
+        <v>80</v>
+      </c>
+      <c r="G24" s="8">
+        <v>0.08</v>
+      </c>
+      <c r="H24" s="13">
+        <f>G24*F24</f>
+        <v>6.4</v>
+      </c>
     </row>
     <row r="25" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D25" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="F25" s="8">
         <v>36</v>
@@ -1339,272 +1440,368 @@
     </row>
     <row r="26" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="7" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="D26" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="F26" s="8">
         <v>24</v>
       </c>
       <c r="G26" s="8">
-        <v>0.08</v>
+        <v>0.31</v>
       </c>
       <c r="H26" s="13">
         <f t="shared" si="1"/>
-        <v>1.92</v>
+        <v>7.4399999999999995</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27" s="8">
-        <v>1714971</v>
+        <v>73</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="D27" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="F27" s="8">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G27" s="8">
-        <v>1.39</v>
+        <v>0.25</v>
       </c>
       <c r="H27" s="13">
         <f t="shared" si="1"/>
-        <v>2.78</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="8">
-        <v>1714984</v>
+        <v>61</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="D28" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E28" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="F28" s="8">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="G28" s="8">
-        <v>2.04</v>
+        <v>0.08</v>
       </c>
       <c r="H28" s="13">
         <f t="shared" si="1"/>
-        <v>2.04</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C29" s="8">
-        <v>1827907</v>
+        <v>67</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="D29" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E29" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="F29" s="8">
-        <v>1</v>
-      </c>
-      <c r="G29" s="8">
-        <v>2.88</v>
+        <v>16</v>
+      </c>
+      <c r="G29" s="13">
+        <v>0.53</v>
       </c>
       <c r="H29" s="13">
         <f t="shared" si="1"/>
-        <v>2.88</v>
+        <v>8.48</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="8">
-        <v>1827745</v>
+        <v>74</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>27</v>
       </c>
       <c r="F30" s="8">
-        <v>1</v>
-      </c>
-      <c r="G30" s="8">
-        <v>4.91</v>
+        <v>6</v>
+      </c>
+      <c r="G30" s="13">
+        <v>2.42</v>
       </c>
       <c r="H30" s="13">
         <f t="shared" si="1"/>
-        <v>4.91</v>
+        <v>14.52</v>
       </c>
     </row>
     <row r="31" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
+      </c>
+      <c r="C31" s="8">
+        <v>1714971</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>27</v>
       </c>
       <c r="F31" s="8">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G31" s="8">
-        <v>17.059999999999999</v>
+        <v>1.39</v>
       </c>
       <c r="H31" s="13">
         <f t="shared" si="1"/>
-        <v>204.71999999999997</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F32" s="3">
-        <v>3</v>
-      </c>
-      <c r="G32" s="3">
-        <v>4.8</v>
+        <v>6.9499999999999993</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="8">
+        <v>1714984</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" s="8">
+        <v>1</v>
+      </c>
+      <c r="G32" s="8">
+        <v>2.04</v>
       </c>
       <c r="H32" s="13">
         <f t="shared" si="1"/>
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="8">
+        <v>1827907</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F33" s="8">
+        <v>1</v>
+      </c>
+      <c r="G33" s="8">
+        <v>2.88</v>
+      </c>
+      <c r="H33" s="13">
+        <f t="shared" si="1"/>
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="8">
+        <v>1827745</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34" s="8">
+        <v>1</v>
+      </c>
+      <c r="G34" s="8">
+        <v>4.91</v>
+      </c>
+      <c r="H34" s="13">
+        <f t="shared" si="1"/>
+        <v>4.91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F35" s="15">
+        <v>12</v>
+      </c>
+      <c r="G35" s="15">
+        <v>17.059999999999999</v>
+      </c>
+      <c r="H35" s="15">
+        <f t="shared" si="1"/>
+        <v>204.71999999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F36" s="3">
+        <v>3</v>
+      </c>
+      <c r="G36" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="H36" s="13">
+        <f t="shared" si="1"/>
         <v>14.399999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-    </row>
-    <row r="34" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="11" t="s">
+    <row r="37" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+    </row>
+    <row r="38" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B38" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C38" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D38" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E38" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="F38" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G34" s="6" t="s">
+      <c r="G38" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H34" s="6" t="s">
+      <c r="H38" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="7" t="s">
+    <row r="39" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8">
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8">
         <v>3</v>
       </c>
-      <c r="G35" s="8"/>
-      <c r="H35" s="13">
-        <f t="shared" ref="H35:H37" si="2">G35*F35</f>
+      <c r="G39" s="8"/>
+      <c r="H39" s="13">
+        <f t="shared" ref="H39:H41" si="2">G39*F39</f>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="7" t="s">
+    <row r="40" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8">
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8">
         <v>3</v>
       </c>
-      <c r="G36" s="8"/>
-      <c r="H36" s="13">
+      <c r="G40" s="8"/>
+      <c r="H40" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="7" t="s">
+    <row r="41" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C41" s="8">
         <v>1714984</v>
       </c>
-      <c r="D37" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E37" s="8" t="s">
+      <c r="D41" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E41" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F37" s="8">
+      <c r="F41" s="8">
         <v>1</v>
       </c>
-      <c r="G37" s="8">
+      <c r="G41" s="8">
         <v>2.04</v>
       </c>
-      <c r="H37" s="13">
+      <c r="H41" s="13">
         <f t="shared" si="2"/>
         <v>2.04</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="12" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="11">
-        <f>SUM(H4:H10)+SUM(H13:H32)+SUM(H35:H37)</f>
-        <v>702.3</v>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="11">
+        <f>SUM(H4:H10)+SUM(H13:H36)+SUM(H39:H41)</f>
+        <v>761.86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>